<commit_message>
now it removes unnecessary junk from the stationid column
</commit_message>
<xml_diff>
--- a/output/blm_swampformat_Dec.xlsx
+++ b/output/blm_swampformat_Dec.xlsx
@@ -454,7 +454,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
     <col width="28" customWidth="1" min="2" max="2"/>
     <col width="24" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
@@ -503,7 +503,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
@@ -538,7 +538,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -568,7 +568,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
@@ -598,7 +598,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
@@ -633,7 +633,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -663,7 +663,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
@@ -693,7 +693,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -723,7 +723,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
@@ -774,7 +774,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
     <col width="28" customWidth="1" min="2" max="2"/>
     <col width="24" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
@@ -841,7 +841,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
@@ -886,7 +886,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -926,7 +926,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
@@ -966,7 +966,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
@@ -1016,7 +1016,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -1061,7 +1061,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
@@ -1101,7 +1101,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -1141,7 +1141,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
@@ -1202,7 +1202,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
     <col width="28" customWidth="1" min="2" max="2"/>
     <col width="24" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
@@ -1263,7 +1263,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
@@ -1308,7 +1308,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -1348,7 +1348,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
@@ -1388,7 +1388,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
@@ -1433,7 +1433,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -1473,7 +1473,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
@@ -1513,7 +1513,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -1553,7 +1553,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
@@ -1598,7 +1598,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
@@ -1643,7 +1643,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
@@ -1683,7 +1683,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
@@ -1723,7 +1723,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
@@ -1768,7 +1768,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
@@ -1808,7 +1808,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
@@ -1848,7 +1848,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
@@ -1888,7 +1888,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
@@ -1949,7 +1949,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
     <col width="28" customWidth="1" min="2" max="2"/>
     <col width="24" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
@@ -2178,7 +2178,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
@@ -2337,7 +2337,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -2491,7 +2491,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
@@ -2645,7 +2645,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
@@ -2804,7 +2804,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -2958,7 +2958,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
@@ -3112,7 +3112,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -3261,7 +3261,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
@@ -3436,7 +3436,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
     <col width="28" customWidth="1" min="2" max="2"/>
     <col width="24" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
@@ -3623,7 +3623,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
@@ -3738,7 +3738,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -3853,7 +3853,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
@@ -3968,7 +3968,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
@@ -4083,7 +4083,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -4198,7 +4198,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
@@ -4313,7 +4313,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -4423,7 +4423,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
@@ -4533,7 +4533,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
@@ -4643,7 +4643,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
@@ -4753,7 +4753,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
@@ -4863,7 +4863,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
@@ -4978,7 +4978,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
@@ -5093,7 +5093,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
@@ -5208,7 +5208,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
@@ -5323,7 +5323,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
@@ -5438,7 +5438,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
@@ -5553,7 +5553,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
@@ -5668,7 +5668,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
@@ -5778,7 +5778,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
@@ -5893,7 +5893,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
@@ -6008,7 +6008,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
@@ -6123,7 +6123,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
@@ -6238,7 +6238,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
@@ -6353,7 +6353,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
@@ -6468,7 +6468,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
@@ -6583,7 +6583,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
@@ -6693,7 +6693,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
@@ -6803,7 +6803,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
@@ -6913,7 +6913,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
@@ -7023,7 +7023,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
@@ -7133,7 +7133,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
@@ -7248,7 +7248,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
@@ -7363,7 +7363,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
@@ -7478,7 +7478,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
@@ -7593,7 +7593,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
@@ -7708,7 +7708,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
@@ -7823,7 +7823,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
@@ -7933,7 +7933,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
@@ -8048,7 +8048,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
@@ -8163,7 +8163,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
@@ -8273,7 +8273,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
@@ -8383,7 +8383,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
@@ -8493,7 +8493,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
@@ -8603,7 +8603,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
@@ -8708,7 +8708,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B47" s="2" t="n">
@@ -8813,7 +8813,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
@@ -8918,7 +8918,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B49" s="2" t="n">
@@ -9023,7 +9023,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B50" s="2" t="n">
@@ -9128,7 +9128,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B51" s="2" t="n">
@@ -9238,7 +9238,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B52" s="2" t="n">
@@ -9348,7 +9348,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B53" s="2" t="n">
@@ -9458,7 +9458,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B54" s="2" t="n">
@@ -9568,7 +9568,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B55" s="2" t="n">
@@ -9678,7 +9678,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B56" s="2" t="n">
@@ -9788,7 +9788,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B57" s="2" t="n">
@@ -9893,7 +9893,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B58" s="2" t="n">
@@ -10003,7 +10003,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B59" s="2" t="n">
@@ -10113,7 +10113,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B60" s="2" t="n">
@@ -10228,7 +10228,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B61" s="2" t="n">
@@ -10343,7 +10343,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B62" s="2" t="n">
@@ -10458,7 +10458,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B63" s="2" t="n">
@@ -10573,7 +10573,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B64" s="2" t="n">
@@ -10683,7 +10683,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B65" s="2" t="n">
@@ -10793,7 +10793,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B66" s="2" t="n">
@@ -10903,7 +10903,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B67" s="2" t="n">
@@ -11013,7 +11013,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B68" s="2" t="n">
@@ -11123,7 +11123,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B69" s="2" t="n">
@@ -11238,7 +11238,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B70" s="2" t="n">
@@ -11353,7 +11353,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B71" s="2" t="n">
@@ -11468,7 +11468,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B72" s="2" t="n">
@@ -11583,7 +11583,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B73" s="2" t="n">
@@ -11698,7 +11698,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B74" s="2" t="n">
@@ -11813,7 +11813,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B75" s="2" t="n">
@@ -11923,7 +11923,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B76" s="2" t="n">
@@ -12038,7 +12038,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B77" s="2" t="n">
@@ -12153,7 +12153,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B78" s="2" t="n">
@@ -12268,7 +12268,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B79" s="2" t="n">
@@ -12383,7 +12383,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B80" s="2" t="n">
@@ -12498,7 +12498,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B81" s="2" t="n">
@@ -12613,7 +12613,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B82" s="2" t="n">
@@ -12723,7 +12723,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B83" s="2" t="n">
@@ -12833,7 +12833,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B84" s="2" t="n">
@@ -12943,7 +12943,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B85" s="2" t="n">
@@ -13053,7 +13053,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B86" s="2" t="n">
@@ -13163,7 +13163,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B87" s="2" t="n">
@@ -13278,7 +13278,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B88" s="2" t="n">
@@ -13393,7 +13393,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B89" s="2" t="n">
@@ -13508,7 +13508,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B90" s="2" t="n">
@@ -13623,7 +13623,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B91" s="2" t="n">
@@ -13738,7 +13738,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B92" s="2" t="n">
@@ -13853,7 +13853,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B93" s="2" t="n">
@@ -13963,7 +13963,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B94" s="2" t="n">
@@ -14078,7 +14078,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B95" s="2" t="n">
@@ -14193,7 +14193,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B96" s="2" t="n">
@@ -14303,7 +14303,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B97" s="2" t="n">
@@ -14413,7 +14413,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B98" s="2" t="n">
@@ -14523,7 +14523,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B99" s="2" t="n">
@@ -14633,7 +14633,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B100" s="2" t="n">
@@ -14738,7 +14738,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B101" s="2" t="n">
@@ -14843,7 +14843,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B102" s="2" t="n">
@@ -14948,7 +14948,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B103" s="2" t="n">
@@ -15053,7 +15053,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B104" s="2" t="n">
@@ -15158,7 +15158,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B105" s="2" t="n">
@@ -15268,7 +15268,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B106" s="2" t="n">
@@ -15378,7 +15378,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B107" s="2" t="n">
@@ -15488,7 +15488,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B108" s="2" t="n">
@@ -15598,7 +15598,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B109" s="2" t="n">
@@ -15708,7 +15708,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B110" s="2" t="n">
@@ -15818,7 +15818,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B111" s="2" t="n">
@@ -15923,7 +15923,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B112" s="2" t="n">
@@ -16033,7 +16033,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B113" s="2" t="n">
@@ -16143,7 +16143,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B114" s="2" t="n">
@@ -16258,7 +16258,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B115" s="2" t="n">
@@ -16373,7 +16373,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B116" s="2" t="n">
@@ -16488,7 +16488,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B117" s="2" t="n">
@@ -16603,7 +16603,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B118" s="2" t="n">
@@ -16713,7 +16713,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B119" s="2" t="n">
@@ -16823,7 +16823,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B120" s="2" t="n">
@@ -16933,7 +16933,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B121" s="2" t="n">
@@ -17043,7 +17043,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B122" s="2" t="n">
@@ -17153,7 +17153,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B123" s="2" t="n">
@@ -17268,7 +17268,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B124" s="2" t="n">
@@ -17383,7 +17383,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B125" s="2" t="n">
@@ -17498,7 +17498,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B126" s="2" t="n">
@@ -17613,7 +17613,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B127" s="2" t="n">
@@ -17728,7 +17728,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B128" s="2" t="n">
@@ -17843,7 +17843,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B129" s="2" t="n">
@@ -17953,7 +17953,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B130" s="2" t="n">
@@ -18068,7 +18068,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B131" s="2" t="n">
@@ -18183,7 +18183,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B132" s="2" t="n">
@@ -18298,7 +18298,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B133" s="2" t="n">
@@ -18413,7 +18413,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B134" s="2" t="n">
@@ -18528,7 +18528,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B135" s="2" t="n">
@@ -18643,7 +18643,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B136" s="2" t="n">
@@ -18753,7 +18753,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B137" s="2" t="n">
@@ -18863,7 +18863,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B138" s="2" t="n">
@@ -18973,7 +18973,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B139" s="2" t="n">
@@ -19083,7 +19083,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B140" s="2" t="n">
@@ -19193,7 +19193,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B141" s="2" t="n">
@@ -19308,7 +19308,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B142" s="2" t="n">
@@ -19423,7 +19423,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B143" s="2" t="n">
@@ -19538,7 +19538,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B144" s="2" t="n">
@@ -19653,7 +19653,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B145" s="2" t="n">
@@ -19768,7 +19768,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B146" s="2" t="n">
@@ -19883,7 +19883,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B147" s="2" t="n">
@@ -19993,7 +19993,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B148" s="2" t="n">
@@ -20108,7 +20108,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B149" s="2" t="n">
@@ -20239,7 +20239,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
     <col width="28" customWidth="1" min="2" max="2"/>
     <col width="24" customWidth="1" min="3" max="3"/>
     <col width="11" customWidth="1" min="4" max="4"/>
@@ -20402,7 +20402,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
@@ -20503,7 +20503,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -20604,7 +20604,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
@@ -20705,7 +20705,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
@@ -20806,7 +20806,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -20907,7 +20907,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
@@ -21008,7 +21008,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -21109,7 +21109,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
@@ -21210,7 +21210,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
@@ -21311,7 +21311,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
@@ -21412,7 +21412,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
@@ -21513,7 +21513,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
@@ -21614,7 +21614,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC1-Fax</t>
+          <t>BC1-Fax</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
@@ -21715,7 +21715,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
@@ -21816,7 +21816,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
@@ -21917,7 +21917,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
@@ -22018,7 +22018,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
@@ -22119,7 +22119,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
@@ -22220,7 +22220,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
@@ -22321,7 +22321,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
@@ -22422,7 +22422,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
@@ -22523,7 +22523,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
@@ -22624,7 +22624,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
@@ -22725,7 +22725,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
@@ -22826,7 +22826,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
@@ -22927,7 +22927,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BLM-RB4-BC2-Ing</t>
+          <t>BC2-Ing</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
@@ -23028,7 +23028,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
@@ -23124,7 +23124,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
@@ -23220,7 +23220,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
@@ -23316,7 +23316,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
@@ -23412,7 +23412,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
@@ -23508,7 +23508,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
@@ -23604,7 +23604,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
@@ -23700,7 +23700,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
@@ -23796,7 +23796,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
@@ -23892,7 +23892,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
@@ -23988,7 +23988,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
@@ -24084,7 +24084,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
@@ -24180,7 +24180,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Art</t>
+          <t>SGR1-Art</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
@@ -24276,7 +24276,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
@@ -24377,7 +24377,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
@@ -24478,7 +24478,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
@@ -24579,7 +24579,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
@@ -24680,7 +24680,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
@@ -24781,7 +24781,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
@@ -24882,7 +24882,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B47" s="2" t="n">
@@ -24983,7 +24983,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
@@ -25084,7 +25084,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B49" s="2" t="n">
@@ -25185,7 +25185,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B50" s="2" t="n">
@@ -25286,7 +25286,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B51" s="2" t="n">
@@ -25387,7 +25387,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B52" s="2" t="n">
@@ -25488,7 +25488,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR1-Est</t>
+          <t>SGR1-Est</t>
         </is>
       </c>
       <c r="B53" s="2" t="n">
@@ -25589,7 +25589,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B54" s="2" t="n">
@@ -25690,7 +25690,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B55" s="2" t="n">
@@ -25791,7 +25791,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B56" s="2" t="n">
@@ -25892,7 +25892,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B57" s="2" t="n">
@@ -25993,7 +25993,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B58" s="2" t="n">
@@ -26094,7 +26094,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B59" s="2" t="n">
@@ -26195,7 +26195,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B60" s="2" t="n">
@@ -26296,7 +26296,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B61" s="2" t="n">
@@ -26397,7 +26397,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B62" s="2" t="n">
@@ -26498,7 +26498,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B63" s="2" t="n">
@@ -26599,7 +26599,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B64" s="2" t="n">
@@ -26700,7 +26700,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B65" s="2" t="n">
@@ -26801,7 +26801,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Fir</t>
+          <t>SGR2-Fir</t>
         </is>
       </c>
       <c r="B66" s="2" t="n">
@@ -26902,7 +26902,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B67" s="2" t="n">
@@ -26998,7 +26998,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B68" s="2" t="n">
@@ -27094,7 +27094,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B69" s="2" t="n">
@@ -27190,7 +27190,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B70" s="2" t="n">
@@ -27286,7 +27286,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B71" s="2" t="n">
@@ -27382,7 +27382,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B72" s="2" t="n">
@@ -27478,7 +27478,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B73" s="2" t="n">
@@ -27574,7 +27574,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B74" s="2" t="n">
@@ -27670,7 +27670,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B75" s="2" t="n">
@@ -27766,7 +27766,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B76" s="2" t="n">
@@ -27862,7 +27862,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B77" s="2" t="n">
@@ -27958,7 +27958,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B78" s="2" t="n">
@@ -28054,7 +28054,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR2-Wht</t>
+          <t>SGR2-Wht</t>
         </is>
       </c>
       <c r="B79" s="2" t="n">
@@ -28150,7 +28150,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B80" s="2" t="n">
@@ -28251,7 +28251,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B81" s="2" t="n">
@@ -28352,7 +28352,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B82" s="2" t="n">
@@ -28453,7 +28453,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B83" s="2" t="n">
@@ -28554,7 +28554,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B84" s="2" t="n">
@@ -28655,7 +28655,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B85" s="2" t="n">
@@ -28756,7 +28756,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B86" s="2" t="n">
@@ -28857,7 +28857,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B87" s="2" t="n">
@@ -28958,7 +28958,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B88" s="2" t="n">
@@ -29059,7 +29059,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B89" s="2" t="n">
@@ -29160,7 +29160,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B90" s="2" t="n">
@@ -29261,7 +29261,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B91" s="2" t="n">
@@ -29362,7 +29362,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Dam</t>
+          <t>SGR3-Dam</t>
         </is>
       </c>
       <c r="B92" s="2" t="n">
@@ -29463,7 +29463,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B93" s="2" t="n">
@@ -29564,7 +29564,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B94" s="2" t="n">
@@ -29665,7 +29665,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B95" s="2" t="n">
@@ -29766,7 +29766,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B96" s="2" t="n">
@@ -29867,7 +29867,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B97" s="2" t="n">
@@ -29968,7 +29968,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B98" s="2" t="n">
@@ -30069,7 +30069,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B99" s="2" t="n">
@@ -30170,7 +30170,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B100" s="2" t="n">
@@ -30271,7 +30271,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B101" s="2" t="n">
@@ -30372,7 +30372,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B102" s="2" t="n">
@@ -30473,7 +30473,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B103" s="2" t="n">
@@ -30574,7 +30574,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B104" s="2" t="n">
@@ -30675,7 +30675,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>BLM-RB4-SGR3-Sjc</t>
+          <t>SGR3-Sjc</t>
         </is>
       </c>
       <c r="B105" s="2" t="n">

</xml_diff>

<commit_message>
reformats just about everything SWAMP wants, just leaves a few duplicate entries, not sure why yet.
</commit_message>
<xml_diff>
--- a/output/blm_swampformat_Dec.xlsx
+++ b/output/blm_swampformat_Dec.xlsx
@@ -12,6 +12,9 @@
     <sheet name="Locations" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="FieldResults" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="HabitatResults" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="BenthicResults" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="ChemResults" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="LabBatch" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -21,7 +24,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -1004,7 +1007,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Dry_NoWater_</t>
+          <t>Dry (no water)</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -1179,7 +1182,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Dry_NoWater_</t>
+          <t>Dry (no water)</t>
         </is>
       </c>
     </row>
@@ -1966,7 +1969,7 @@
     <col width="17" customWidth="1" min="15" max="15"/>
     <col width="19" customWidth="1" min="16" max="16"/>
     <col width="23" customWidth="1" min="17" max="17"/>
-    <col width="16" customWidth="1" min="18" max="18"/>
+    <col width="10" customWidth="1" min="18" max="18"/>
     <col width="13" customWidth="1" min="19" max="19"/>
     <col width="26" customWidth="1" min="20" max="20"/>
     <col width="18" customWidth="1" min="21" max="21"/>
@@ -1983,7 +1986,7 @@
     <col width="15" customWidth="1" min="32" max="32"/>
     <col width="14" customWidth="1" min="33" max="33"/>
     <col width="16" customWidth="1" min="34" max="34"/>
-    <col width="18" customWidth="1" min="35" max="35"/>
+    <col width="21" customWidth="1" min="35" max="35"/>
     <col width="12" customWidth="1" min="36" max="36"/>
     <col width="18" customWidth="1" min="37" max="37"/>
   </cols>
@@ -2255,7 +2258,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>ConcretChannel</t>
+          <t>ConChan</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -2269,7 +2272,7 @@
         </is>
       </c>
       <c r="V2" t="n">
-        <v>-88</v>
+        <v>1</v>
       </c>
       <c r="W2" t="n">
         <v>33.9894758333333</v>
@@ -2323,10 +2326,8 @@
           <t>DarioDiehl</t>
         </is>
       </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>2020-12-15</t>
-        </is>
+      <c r="AI2" s="2" t="n">
+        <v>44180</v>
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
@@ -2409,7 +2410,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>ConcretChannel</t>
+          <t>ConChan</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -2423,7 +2424,7 @@
         </is>
       </c>
       <c r="V3" t="n">
-        <v>-88</v>
+        <v>1</v>
       </c>
       <c r="W3" t="n">
         <v>34.0385098333333</v>
@@ -2477,10 +2478,8 @@
           <t>DarioDiehl</t>
         </is>
       </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>2020-12-15</t>
-        </is>
+      <c r="AI3" s="2" t="n">
+        <v>44180</v>
       </c>
       <c r="AJ3" t="inlineStr">
         <is>
@@ -2563,7 +2562,7 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Dyke_Levee</t>
+          <t>Dam</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -2577,7 +2576,7 @@
         </is>
       </c>
       <c r="V4" t="n">
-        <v>-88</v>
+        <v>1</v>
       </c>
       <c r="W4" t="n">
         <v>34.0388481666667</v>
@@ -2631,10 +2630,8 @@
           <t>DarioDiehl</t>
         </is>
       </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>2020-12-15</t>
-        </is>
+      <c r="AI4" s="2" t="n">
+        <v>44180</v>
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
@@ -2736,7 +2733,7 @@
         </is>
       </c>
       <c r="V5" t="n">
-        <v>-88</v>
+        <v>1</v>
       </c>
       <c r="W5" t="n">
         <v>34.022396</v>
@@ -2790,10 +2787,8 @@
           <t>DarioDiehl</t>
         </is>
       </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>2020-12-15</t>
-        </is>
+      <c r="AI5" s="2" t="n">
+        <v>44180</v>
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
@@ -2876,7 +2871,7 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>Dyke_Levee</t>
+          <t>Weir</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -2890,7 +2885,7 @@
         </is>
       </c>
       <c r="V6" t="n">
-        <v>-88</v>
+        <v>1</v>
       </c>
       <c r="W6" t="n">
         <v>33.993916</v>
@@ -2944,10 +2939,8 @@
           <t>DarioDiehl</t>
         </is>
       </c>
-      <c r="AI6" t="inlineStr">
-        <is>
-          <t>2020-12-15</t>
-        </is>
+      <c r="AI6" s="2" t="n">
+        <v>44180</v>
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
@@ -3030,7 +3023,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>ConcretChannel</t>
+          <t>ConChan</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -3044,7 +3037,7 @@
         </is>
       </c>
       <c r="V7" t="n">
-        <v>-88</v>
+        <v>1</v>
       </c>
       <c r="W7" t="n">
         <v>33.8709558333333</v>
@@ -3098,10 +3091,8 @@
           <t>DarioDiehl</t>
         </is>
       </c>
-      <c r="AI7" t="inlineStr">
-        <is>
-          <t>2020-12-15</t>
-        </is>
+      <c r="AI7" s="2" t="n">
+        <v>44180</v>
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
@@ -3179,7 +3170,7 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>ConcretChannel</t>
+          <t>ConChan</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -3193,7 +3184,7 @@
         </is>
       </c>
       <c r="V8" t="n">
-        <v>-88</v>
+        <v>1</v>
       </c>
       <c r="W8" t="n">
         <v>33.7910585</v>
@@ -3247,10 +3238,8 @@
           <t>DarioDiehl</t>
         </is>
       </c>
-      <c r="AI8" t="inlineStr">
-        <is>
-          <t>2020-12-15</t>
-        </is>
+      <c r="AI8" s="2" t="n">
+        <v>44180</v>
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
@@ -3338,7 +3327,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>ConcretChannel</t>
+          <t>ConChan</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -3352,7 +3341,7 @@
         </is>
       </c>
       <c r="V9" t="n">
-        <v>-88</v>
+        <v>1</v>
       </c>
       <c r="W9" t="n">
         <v>33.9295635</v>
@@ -3406,10 +3395,8 @@
           <t>DarioDiehl</t>
         </is>
       </c>
-      <c r="AI9" t="inlineStr">
-        <is>
-          <t>2020-12-15</t>
-        </is>
+      <c r="AI9" s="2" t="n">
+        <v>44180</v>
       </c>
       <c r="AJ9" t="inlineStr">
         <is>
@@ -3712,7 +3699,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>mg_L</t>
+          <t>mg/L</t>
         </is>
       </c>
       <c r="V2" t="n">
@@ -3728,7 +3715,7 @@
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC2" s="2" t="n">
@@ -3827,7 +3814,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>mg_L</t>
+          <t>mg/L</t>
         </is>
       </c>
       <c r="V3" t="n">
@@ -3843,7 +3830,7 @@
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC3" s="2" t="n">
@@ -3942,7 +3929,7 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>percent</t>
+          <t>%</t>
         </is>
       </c>
       <c r="V4" t="n">
@@ -3958,7 +3945,7 @@
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC4" s="2" t="n">
@@ -4057,7 +4044,7 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>percent</t>
+          <t>%</t>
         </is>
       </c>
       <c r="V5" t="n">
@@ -4073,7 +4060,7 @@
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC5" s="2" t="n">
@@ -4188,7 +4175,7 @@
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC6" s="2" t="n">
@@ -4287,7 +4274,7 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>µS_cm</t>
+          <t>uS/cm</t>
         </is>
       </c>
       <c r="V7" t="n">
@@ -4303,7 +4290,7 @@
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC7" s="2" t="n">
@@ -4416,6 +4403,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC8" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -4526,6 +4518,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC9" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -4636,6 +4633,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC10" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -4746,6 +4748,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC11" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -4856,6 +4863,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC12" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -4952,7 +4964,7 @@
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>degreeC</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V13" t="n">
@@ -5067,7 +5079,7 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>degree C</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V14" t="n">
@@ -5083,7 +5095,7 @@
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC14" s="2" t="n">
@@ -5182,7 +5194,7 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>degree C</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V15" t="n">
@@ -5198,7 +5210,7 @@
       </c>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC15" s="2" t="n">
@@ -5297,7 +5309,7 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V16" t="n">
@@ -5313,7 +5325,7 @@
       </c>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC16" s="2" t="n">
@@ -5412,7 +5424,7 @@
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V17" t="n">
@@ -5428,7 +5440,7 @@
       </c>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC17" s="2" t="n">
@@ -5527,7 +5539,7 @@
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V18" t="n">
@@ -5543,7 +5555,7 @@
       </c>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC18" s="2" t="n">
@@ -5642,7 +5654,7 @@
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V19" t="n">
@@ -5658,7 +5670,7 @@
       </c>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC19" s="2" t="n">
@@ -5771,6 +5783,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC20" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -5867,7 +5884,7 @@
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V21" t="n">
@@ -5998,7 +6015,7 @@
       </c>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC22" s="2" t="n">
@@ -6113,7 +6130,7 @@
       </c>
       <c r="AB23" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC23" s="2" t="n">
@@ -6212,7 +6229,7 @@
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>mg_L</t>
+          <t>mg/L</t>
         </is>
       </c>
       <c r="V24" t="n">
@@ -6228,7 +6245,7 @@
       </c>
       <c r="AB24" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC24" s="2" t="n">
@@ -6327,7 +6344,7 @@
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>percent</t>
+          <t>%</t>
         </is>
       </c>
       <c r="V25" t="n">
@@ -6343,7 +6360,7 @@
       </c>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC25" s="2" t="n">
@@ -6458,7 +6475,7 @@
       </c>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC26" s="2" t="n">
@@ -6557,7 +6574,7 @@
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>µS_cm</t>
+          <t>uS/cm</t>
         </is>
       </c>
       <c r="V27" t="n">
@@ -6573,7 +6590,7 @@
       </c>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC27" s="2" t="n">
@@ -6686,6 +6703,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC28" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -6796,6 +6818,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC29" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -6906,6 +6933,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC30" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -7016,6 +7048,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC31" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -7126,6 +7163,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC32" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -7222,7 +7264,7 @@
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>degreeC</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V33" t="n">
@@ -7337,7 +7379,7 @@
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>degree C</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V34" t="n">
@@ -7353,7 +7395,7 @@
       </c>
       <c r="AB34" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC34" s="2" t="n">
@@ -7452,7 +7494,7 @@
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V35" t="n">
@@ -7468,7 +7510,7 @@
       </c>
       <c r="AB35" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC35" s="2" t="n">
@@ -7567,7 +7609,7 @@
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V36" t="n">
@@ -7583,7 +7625,7 @@
       </c>
       <c r="AB36" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC36" s="2" t="n">
@@ -7682,7 +7724,7 @@
       </c>
       <c r="U37" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V37" t="n">
@@ -7698,7 +7740,7 @@
       </c>
       <c r="AB37" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC37" s="2" t="n">
@@ -7797,7 +7839,7 @@
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V38" t="n">
@@ -7813,7 +7855,7 @@
       </c>
       <c r="AB38" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC38" s="2" t="n">
@@ -7926,6 +7968,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB39" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC39" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -8022,7 +8069,7 @@
       </c>
       <c r="U40" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V40" t="n">
@@ -8153,7 +8200,7 @@
       </c>
       <c r="AB41" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC41" s="2" t="n">
@@ -8247,7 +8294,7 @@
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>mg_L</t>
+          <t>mg/L</t>
         </is>
       </c>
       <c r="V42" t="n">
@@ -8263,7 +8310,7 @@
       </c>
       <c r="AB42" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC42" s="2" t="n">
@@ -8357,7 +8404,7 @@
       </c>
       <c r="U43" t="inlineStr">
         <is>
-          <t>percent</t>
+          <t>%</t>
         </is>
       </c>
       <c r="V43" t="n">
@@ -8373,7 +8420,7 @@
       </c>
       <c r="AB43" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC43" s="2" t="n">
@@ -8483,7 +8530,7 @@
       </c>
       <c r="AB44" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC44" s="2" t="n">
@@ -8577,7 +8624,7 @@
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>µS_cm</t>
+          <t>uS/cm</t>
         </is>
       </c>
       <c r="V45" t="n">
@@ -8593,7 +8640,7 @@
       </c>
       <c r="AB45" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC45" s="2" t="n">
@@ -8701,6 +8748,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB46" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC46" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -8806,6 +8858,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB47" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC47" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -8911,6 +8968,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB48" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC48" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -9016,6 +9078,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB49" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC49" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -9121,6 +9188,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB50" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC50" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -9212,7 +9284,7 @@
       </c>
       <c r="U51" t="inlineStr">
         <is>
-          <t>degreeC</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V51" t="n">
@@ -9322,7 +9394,7 @@
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>degree C</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V52" t="n">
@@ -9338,7 +9410,7 @@
       </c>
       <c r="AB52" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC52" s="2" t="n">
@@ -9432,7 +9504,7 @@
       </c>
       <c r="U53" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V53" t="n">
@@ -9448,7 +9520,7 @@
       </c>
       <c r="AB53" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC53" s="2" t="n">
@@ -9542,7 +9614,7 @@
       </c>
       <c r="U54" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V54" t="n">
@@ -9558,7 +9630,7 @@
       </c>
       <c r="AB54" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC54" s="2" t="n">
@@ -9652,7 +9724,7 @@
       </c>
       <c r="U55" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V55" t="n">
@@ -9668,7 +9740,7 @@
       </c>
       <c r="AB55" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC55" s="2" t="n">
@@ -9762,7 +9834,7 @@
       </c>
       <c r="U56" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V56" t="n">
@@ -9778,7 +9850,7 @@
       </c>
       <c r="AB56" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC56" s="2" t="n">
@@ -9886,6 +9958,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB57" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC57" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -9977,7 +10054,7 @@
       </c>
       <c r="U58" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V58" t="n">
@@ -10103,7 +10180,7 @@
       </c>
       <c r="AB59" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC59" s="2" t="n">
@@ -10202,7 +10279,7 @@
       </c>
       <c r="U60" t="inlineStr">
         <is>
-          <t>mg_L</t>
+          <t>mg/L</t>
         </is>
       </c>
       <c r="V60" t="n">
@@ -10218,7 +10295,7 @@
       </c>
       <c r="AB60" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC60" s="2" t="n">
@@ -10317,7 +10394,7 @@
       </c>
       <c r="U61" t="inlineStr">
         <is>
-          <t>percent</t>
+          <t>%</t>
         </is>
       </c>
       <c r="V61" t="n">
@@ -10333,7 +10410,7 @@
       </c>
       <c r="AB61" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC61" s="2" t="n">
@@ -10448,7 +10525,7 @@
       </c>
       <c r="AB62" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC62" s="2" t="n">
@@ -10547,7 +10624,7 @@
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>µS_cm</t>
+          <t>uS/cm</t>
         </is>
       </c>
       <c r="V63" t="n">
@@ -10563,7 +10640,7 @@
       </c>
       <c r="AB63" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC63" s="2" t="n">
@@ -10676,6 +10753,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB64" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC64" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -10786,6 +10868,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB65" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC65" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -10896,6 +10983,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB66" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC66" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -11006,6 +11098,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB67" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC67" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -11116,6 +11213,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB68" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC68" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -11212,7 +11314,7 @@
       </c>
       <c r="U69" t="inlineStr">
         <is>
-          <t>degreeC</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V69" t="n">
@@ -11327,7 +11429,7 @@
       </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>degree C</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V70" t="n">
@@ -11343,7 +11445,7 @@
       </c>
       <c r="AB70" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC70" s="2" t="n">
@@ -11442,7 +11544,7 @@
       </c>
       <c r="U71" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V71" t="n">
@@ -11458,7 +11560,7 @@
       </c>
       <c r="AB71" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC71" s="2" t="n">
@@ -11557,7 +11659,7 @@
       </c>
       <c r="U72" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V72" t="n">
@@ -11573,7 +11675,7 @@
       </c>
       <c r="AB72" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC72" s="2" t="n">
@@ -11672,7 +11774,7 @@
       </c>
       <c r="U73" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V73" t="n">
@@ -11688,7 +11790,7 @@
       </c>
       <c r="AB73" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC73" s="2" t="n">
@@ -11787,7 +11889,7 @@
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V74" t="n">
@@ -11803,7 +11905,7 @@
       </c>
       <c r="AB74" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC74" s="2" t="n">
@@ -11916,6 +12018,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB75" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC75" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -12012,7 +12119,7 @@
       </c>
       <c r="U76" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V76" t="n">
@@ -12143,7 +12250,7 @@
       </c>
       <c r="AB77" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC77" s="2" t="n">
@@ -12242,7 +12349,7 @@
       </c>
       <c r="U78" t="inlineStr">
         <is>
-          <t>mg_L</t>
+          <t>mg/L</t>
         </is>
       </c>
       <c r="V78" t="n">
@@ -12258,7 +12365,7 @@
       </c>
       <c r="AB78" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC78" s="2" t="n">
@@ -12357,7 +12464,7 @@
       </c>
       <c r="U79" t="inlineStr">
         <is>
-          <t>percent</t>
+          <t>%</t>
         </is>
       </c>
       <c r="V79" t="n">
@@ -12373,7 +12480,7 @@
       </c>
       <c r="AB79" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC79" s="2" t="n">
@@ -12488,7 +12595,7 @@
       </c>
       <c r="AB80" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC80" s="2" t="n">
@@ -12587,7 +12694,7 @@
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>µS_cm</t>
+          <t>uS/cm</t>
         </is>
       </c>
       <c r="V81" t="n">
@@ -12603,7 +12710,7 @@
       </c>
       <c r="AB81" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC81" s="2" t="n">
@@ -12716,6 +12823,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB82" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC82" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -12826,6 +12938,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB83" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC83" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -12936,6 +13053,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB84" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC84" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -13046,6 +13168,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB85" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC85" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -13156,6 +13283,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB86" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC86" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -13252,7 +13384,7 @@
       </c>
       <c r="U87" t="inlineStr">
         <is>
-          <t>degreeC</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V87" t="n">
@@ -13367,7 +13499,7 @@
       </c>
       <c r="U88" t="inlineStr">
         <is>
-          <t>degree C</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V88" t="n">
@@ -13383,7 +13515,7 @@
       </c>
       <c r="AB88" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC88" s="2" t="n">
@@ -13498,7 +13630,7 @@
       </c>
       <c r="AB89" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC89" s="2" t="n">
@@ -13613,7 +13745,7 @@
       </c>
       <c r="AB90" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC90" s="2" t="n">
@@ -13728,7 +13860,7 @@
       </c>
       <c r="AB91" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC91" s="2" t="n">
@@ -13843,7 +13975,7 @@
       </c>
       <c r="AB92" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC92" s="2" t="n">
@@ -13956,6 +14088,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB93" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC93" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -14052,7 +14189,7 @@
       </c>
       <c r="U94" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V94" t="n">
@@ -14183,7 +14320,7 @@
       </c>
       <c r="AB95" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC95" s="2" t="n">
@@ -14277,7 +14414,7 @@
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>mg_L</t>
+          <t>mg/L</t>
         </is>
       </c>
       <c r="V96" t="n">
@@ -14293,7 +14430,7 @@
       </c>
       <c r="AB96" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC96" s="2" t="n">
@@ -14387,7 +14524,7 @@
       </c>
       <c r="U97" t="inlineStr">
         <is>
-          <t>percent</t>
+          <t>%</t>
         </is>
       </c>
       <c r="V97" t="n">
@@ -14403,7 +14540,7 @@
       </c>
       <c r="AB97" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC97" s="2" t="n">
@@ -14513,7 +14650,7 @@
       </c>
       <c r="AB98" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC98" s="2" t="n">
@@ -14607,7 +14744,7 @@
       </c>
       <c r="U99" t="inlineStr">
         <is>
-          <t>µS_cm</t>
+          <t>uS/cm</t>
         </is>
       </c>
       <c r="V99" t="n">
@@ -14623,7 +14760,7 @@
       </c>
       <c r="AB99" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC99" s="2" t="n">
@@ -14731,6 +14868,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB100" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC100" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -14836,6 +14978,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB101" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC101" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -14941,6 +15088,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB102" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC102" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -15046,6 +15198,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB103" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC103" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -15151,6 +15308,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB104" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC104" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -15242,7 +15404,7 @@
       </c>
       <c r="U105" t="inlineStr">
         <is>
-          <t>degreeC</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V105" t="n">
@@ -15352,7 +15514,7 @@
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>degree C</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V106" t="n">
@@ -15368,7 +15530,7 @@
       </c>
       <c r="AB106" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC106" s="2" t="n">
@@ -15462,7 +15624,7 @@
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V107" t="n">
@@ -15478,7 +15640,7 @@
       </c>
       <c r="AB107" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC107" s="2" t="n">
@@ -15572,7 +15734,7 @@
       </c>
       <c r="U108" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V108" t="n">
@@ -15588,7 +15750,7 @@
       </c>
       <c r="AB108" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC108" s="2" t="n">
@@ -15682,7 +15844,7 @@
       </c>
       <c r="U109" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V109" t="n">
@@ -15698,7 +15860,7 @@
       </c>
       <c r="AB109" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC109" s="2" t="n">
@@ -15808,7 +15970,7 @@
       </c>
       <c r="AB110" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC110" s="2" t="n">
@@ -15916,6 +16078,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB111" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC111" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -16007,7 +16174,7 @@
       </c>
       <c r="U112" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V112" t="n">
@@ -16133,7 +16300,7 @@
       </c>
       <c r="AB113" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC113" s="2" t="n">
@@ -16232,7 +16399,7 @@
       </c>
       <c r="U114" t="inlineStr">
         <is>
-          <t>mg_L</t>
+          <t>mg/L</t>
         </is>
       </c>
       <c r="V114" t="n">
@@ -16248,7 +16415,7 @@
       </c>
       <c r="AB114" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC114" s="2" t="n">
@@ -16347,7 +16514,7 @@
       </c>
       <c r="U115" t="inlineStr">
         <is>
-          <t>percent</t>
+          <t>%</t>
         </is>
       </c>
       <c r="V115" t="n">
@@ -16363,7 +16530,7 @@
       </c>
       <c r="AB115" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC115" s="2" t="n">
@@ -16478,7 +16645,7 @@
       </c>
       <c r="AB116" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC116" s="2" t="n">
@@ -16577,7 +16744,7 @@
       </c>
       <c r="U117" t="inlineStr">
         <is>
-          <t>µS_cm</t>
+          <t>uS/cm</t>
         </is>
       </c>
       <c r="V117" t="n">
@@ -16593,7 +16760,7 @@
       </c>
       <c r="AB117" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC117" s="2" t="n">
@@ -16706,6 +16873,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB118" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC118" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -16816,6 +16988,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB119" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC119" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -16926,6 +17103,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB120" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC120" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -17036,6 +17218,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB121" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC121" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -17146,6 +17333,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB122" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC122" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -17242,7 +17434,7 @@
       </c>
       <c r="U123" t="inlineStr">
         <is>
-          <t>degreeC</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V123" t="n">
@@ -17357,7 +17549,7 @@
       </c>
       <c r="U124" t="inlineStr">
         <is>
-          <t>degree C</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V124" t="n">
@@ -17373,7 +17565,7 @@
       </c>
       <c r="AB124" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC124" s="2" t="n">
@@ -17488,7 +17680,7 @@
       </c>
       <c r="AB125" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC125" s="2" t="n">
@@ -17603,7 +17795,7 @@
       </c>
       <c r="AB126" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC126" s="2" t="n">
@@ -17718,7 +17910,7 @@
       </c>
       <c r="AB127" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC127" s="2" t="n">
@@ -17833,7 +18025,7 @@
       </c>
       <c r="AB128" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC128" s="2" t="n">
@@ -17946,6 +18138,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB129" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC129" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -18042,7 +18239,7 @@
       </c>
       <c r="U130" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V130" t="n">
@@ -18173,7 +18370,7 @@
       </c>
       <c r="AB131" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC131" s="2" t="n">
@@ -18272,7 +18469,7 @@
       </c>
       <c r="U132" t="inlineStr">
         <is>
-          <t>mg_L</t>
+          <t>mg/L</t>
         </is>
       </c>
       <c r="V132" t="n">
@@ -18288,7 +18485,7 @@
       </c>
       <c r="AB132" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC132" s="2" t="n">
@@ -18387,7 +18584,7 @@
       </c>
       <c r="U133" t="inlineStr">
         <is>
-          <t>percent</t>
+          <t>%</t>
         </is>
       </c>
       <c r="V133" t="n">
@@ -18403,7 +18600,7 @@
       </c>
       <c r="AB133" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC133" s="2" t="n">
@@ -18518,7 +18715,7 @@
       </c>
       <c r="AB134" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC134" s="2" t="n">
@@ -18617,7 +18814,7 @@
       </c>
       <c r="U135" t="inlineStr">
         <is>
-          <t>µS_cm</t>
+          <t>uS/cm</t>
         </is>
       </c>
       <c r="V135" t="n">
@@ -18633,7 +18830,7 @@
       </c>
       <c r="AB135" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC135" s="2" t="n">
@@ -18746,6 +18943,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB136" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC136" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -18856,6 +19058,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB137" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC137" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -18966,6 +19173,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB138" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC138" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -19076,6 +19288,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB139" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC139" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -19186,6 +19403,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB140" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC140" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -19282,7 +19504,7 @@
       </c>
       <c r="U141" t="inlineStr">
         <is>
-          <t>degreeC</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V141" t="n">
@@ -19397,7 +19619,7 @@
       </c>
       <c r="U142" t="inlineStr">
         <is>
-          <t>degree C</t>
+          <t>deg C</t>
         </is>
       </c>
       <c r="V142" t="n">
@@ -19413,7 +19635,7 @@
       </c>
       <c r="AB142" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC142" s="2" t="n">
@@ -19528,7 +19750,7 @@
       </c>
       <c r="AB143" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC143" s="2" t="n">
@@ -19643,7 +19865,7 @@
       </c>
       <c r="AB144" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC144" s="2" t="n">
@@ -19758,7 +19980,7 @@
       </c>
       <c r="AB145" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC145" s="2" t="n">
@@ -19873,7 +20095,7 @@
       </c>
       <c r="AB146" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC146" s="2" t="n">
@@ -19986,6 +20208,11 @@
           <t>=</t>
         </is>
       </c>
+      <c r="AB147" t="inlineStr">
+        <is>
+          <t>Wading Rod</t>
+        </is>
+      </c>
       <c r="AC147" s="2" t="n">
         <v>44179.83333333334</v>
       </c>
@@ -20082,7 +20309,7 @@
       </c>
       <c r="U148" t="inlineStr">
         <is>
-          <t>m_s</t>
+          <t>m/s</t>
         </is>
       </c>
       <c r="V148" t="n">
@@ -20213,7 +20440,7 @@
       </c>
       <c r="AB149" t="inlineStr">
         <is>
-          <t>YSIPro1020</t>
+          <t>YSI Pro1020</t>
         </is>
       </c>
       <c r="AC149" s="2" t="n">
@@ -30776,4 +31003,679 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BB1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="16" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
+    <col width="11" customWidth="1" min="13" max="13"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="11" customWidth="1" min="15" max="15"/>
+    <col width="17" customWidth="1" min="16" max="16"/>
+    <col width="21" customWidth="1" min="17" max="17"/>
+    <col width="10" customWidth="1" min="18" max="18"/>
+    <col width="27" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="14" customWidth="1" min="21" max="21"/>
+    <col width="15" customWidth="1" min="22" max="22"/>
+    <col width="25" customWidth="1" min="23" max="23"/>
+    <col width="12" customWidth="1" min="24" max="24"/>
+    <col width="33" customWidth="1" min="25" max="25"/>
+    <col width="22" customWidth="1" min="26" max="26"/>
+    <col width="25" customWidth="1" min="27" max="27"/>
+    <col width="22" customWidth="1" min="28" max="28"/>
+    <col width="12" customWidth="1" min="29" max="29"/>
+    <col width="15" customWidth="1" min="30" max="30"/>
+    <col width="21" customWidth="1" min="31" max="31"/>
+    <col width="21" customWidth="1" min="32" max="32"/>
+    <col width="21" customWidth="1" min="33" max="33"/>
+    <col width="20" customWidth="1" min="34" max="34"/>
+    <col width="17" customWidth="1" min="35" max="35"/>
+    <col width="24" customWidth="1" min="36" max="36"/>
+    <col width="14" customWidth="1" min="37" max="37"/>
+    <col width="26" customWidth="1" min="38" max="38"/>
+    <col width="9" customWidth="1" min="39" max="39"/>
+    <col width="15" customWidth="1" min="40" max="40"/>
+    <col width="10" customWidth="1" min="41" max="41"/>
+    <col width="10" customWidth="1" min="42" max="42"/>
+    <col width="8" customWidth="1" min="43" max="43"/>
+    <col width="10" customWidth="1" min="44" max="44"/>
+    <col width="13" customWidth="1" min="45" max="45"/>
+    <col width="8" customWidth="1" min="46" max="46"/>
+    <col width="16" customWidth="1" min="47" max="47"/>
+    <col width="23" customWidth="1" min="48" max="48"/>
+    <col width="20" customWidth="1" min="49" max="49"/>
+    <col width="14" customWidth="1" min="50" max="50"/>
+    <col width="22" customWidth="1" min="51" max="51"/>
+    <col width="13" customWidth="1" min="52" max="52"/>
+    <col width="11" customWidth="1" min="53" max="53"/>
+    <col width="23" customWidth="1" min="54" max="54"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>StationCode</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>SampleDate</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ProjectCode</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>EventCode</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ProtocolCode</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>AgencyCode</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>SampleComments</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>LocationCode</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>GeometryShape</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>CollectionTime</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>CollectionMethodCode</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>SampleTypeCode</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Replicate</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>CollectionDeviceName</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>SieveSize</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>CollectionDepth</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>UnitCollectionDepth</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>SampleID</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>BenthicCollectionComments</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>GrabSize</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>UnitGrabSize</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>ReplicateName</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>ReplicateCollectionDate</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>NumberJars</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>BenthicCollectionDetailComments</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>AgencyCode_LabEffort</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>PersonnelCode_LabEffort</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>PercentSampleCounted</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>TotalGrids</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>GridsAnalyzed</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>GridsVolumeAnalyzed</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>TargetOrganismCount</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>ActualOrganismCount</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>ExtraOrganismCount</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>QCOrganismCount</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>DiscardedOrganismCount</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>EffortQACode</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>BenthicLabEffortComments</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>FinalID</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>LifeStageCode</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Distinct</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>BAResult</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>UnitName</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>ResQualCode</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>QACode</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>ComplianceCode</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>BatchVerificationCode</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>TaxonomicQualifier</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>ExcludedTaxa</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>PersonnelCode_Result</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>LabSampleID</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>EnterDate</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>BenthicResultComments</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AO1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="16" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
+    <col width="11" customWidth="1" min="13" max="13"/>
+    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="17" customWidth="1" min="15" max="15"/>
+    <col width="21" customWidth="1" min="16" max="16"/>
+    <col width="21" customWidth="1" min="17" max="17"/>
+    <col width="23" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="12" customWidth="1" min="20" max="20"/>
+    <col width="13" customWidth="1" min="21" max="21"/>
+    <col width="14" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="10" customWidth="1" min="24" max="24"/>
+    <col width="14" customWidth="1" min="25" max="25"/>
+    <col width="10" customWidth="1" min="26" max="26"/>
+    <col width="13" customWidth="1" min="27" max="27"/>
+    <col width="22" customWidth="1" min="28" max="28"/>
+    <col width="22" customWidth="1" min="29" max="29"/>
+    <col width="21" customWidth="1" min="30" max="30"/>
+    <col width="19" customWidth="1" min="31" max="31"/>
+    <col width="14" customWidth="1" min="32" max="32"/>
+    <col width="8" customWidth="1" min="33" max="33"/>
+    <col width="13" customWidth="1" min="34" max="34"/>
+    <col width="5" customWidth="1" min="35" max="35"/>
+    <col width="4" customWidth="1" min="36" max="36"/>
+    <col width="16" customWidth="1" min="37" max="37"/>
+    <col width="8" customWidth="1" min="38" max="38"/>
+    <col width="16" customWidth="1" min="39" max="39"/>
+    <col width="15" customWidth="1" min="40" max="40"/>
+    <col width="19" customWidth="1" min="41" max="41"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>StationCode</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>SampleDate</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ProjectCode</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>EventCode</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ProtocolCode</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>AgencyCode</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>SampleComments</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>LocationCode</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>GeometryShape</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>CollectionTime</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>CollectionMethodCode</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>SampleTypeCode</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Replicate</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>CollectionDeviceName</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>CollectionDepth</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>UnitCollectionDepth</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>PositionWaterColumn</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>LabCollectionComments</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>MatrixName</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>MethodName</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>AnalyteName</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>FractionName</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>UnitName</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>LabBatch</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>AnalysisDate</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>SampleID</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>LabSampleID</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>PrepPreservationName</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>PrepPreservationDate</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>DigestExtractMethod</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>DigestExtractDate</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>LabReplicate</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>ResQualCode</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>MDL</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>RL</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>DilutionFactor</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>QACode</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>ComplianceCode</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>ExpectedValue</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>LabResultComments</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="10" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LabBatch</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>AgencyCode</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>SubmittingAgencyCode</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>LabSubmissionCode</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>BatchVerificationCode</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>LabBatchComments</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>